<commit_message>
Added csv and table handling and special handling for ms office rtf. Am preparing MpDataModelProvider to handle all search criteria.
</commit_message>
<xml_diff>
--- a/SearchNotes.xlsx
+++ b/SearchNotes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="94" windowWidth="17314" windowHeight="7749"/>
+    <workbookView xWindow="480" yWindow="94" windowWidth="17314" windowHeight="7749" tabRatio="269"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -217,13 +217,20 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -243,16 +250,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -545,10 +558,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E130"/>
+  <dimension ref="A1:K130"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6"/>
@@ -560,7 +573,7 @@
     <col min="5" max="5" width="29.4609375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -571,7 +584,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:11">
       <c r="B2" t="s">
         <v>2</v>
       </c>
@@ -579,7 +592,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:11">
       <c r="B3" t="s">
         <v>3</v>
       </c>
@@ -587,7 +600,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:11">
       <c r="B4" t="s">
         <v>4</v>
       </c>
@@ -595,7 +608,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:11">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -609,7 +622,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:11">
       <c r="C7" t="s">
         <v>2</v>
       </c>
@@ -617,15 +630,16 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:11">
       <c r="C8" t="s">
         <v>3</v>
       </c>
       <c r="D8" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="K8" s="2"/>
+    </row>
+    <row r="9" spans="1:11">
       <c r="C9" t="s">
         <v>4</v>
       </c>
@@ -633,7 +647,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:11">
       <c r="B11" t="s">
         <v>8</v>
       </c>
@@ -647,22 +661,22 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:11">
       <c r="E12" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:11">
       <c r="E13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:11">
       <c r="E14" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:11">
       <c r="D15" t="s">
         <v>15</v>
       </c>
@@ -670,7 +684,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:11">
       <c r="E16" t="s">
         <v>12</v>
       </c>

</xml_diff>